<commit_message>
allow multiple file uploads
</commit_message>
<xml_diff>
--- a/File2.xlsx
+++ b/File2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Mini-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E693F27-F98E-4659-9338-3AF7E127ABD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0892E387-F88E-4919-A23E-C1F4340973CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1416" yWindow="996" windowWidth="21624" windowHeight="11244" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>BG</t>
   </si>
@@ -72,46 +72,31 @@
     <t>Status</t>
   </si>
   <si>
-    <t>Averis</t>
-  </si>
-  <si>
-    <t>Averis Sdn</t>
-  </si>
-  <si>
-    <t>BSC Prod H</t>
-  </si>
-  <si>
-    <t>PJR20243G</t>
-  </si>
-  <si>
-    <t>SOWVAV2</t>
-  </si>
-  <si>
-    <t>Allan Teoh Joo Chwan</t>
-  </si>
-  <si>
-    <t>2/15/2024 8:17</t>
-  </si>
-  <si>
-    <t>Projects-IT Infra</t>
-  </si>
-  <si>
-    <t>Completed</t>
-  </si>
-  <si>
-    <t>VMWare V</t>
-  </si>
-  <si>
-    <t>PJR202413</t>
-  </si>
-  <si>
-    <t>Iswani Mustafa</t>
-  </si>
-  <si>
-    <t>5/31/2024 3:44</t>
-  </si>
-  <si>
     <t>In Progress</t>
+  </si>
+  <si>
+    <t>Family Office</t>
+  </si>
+  <si>
+    <t>Pacific Eagle</t>
+  </si>
+  <si>
+    <t>3rd Party Risk</t>
+  </si>
+  <si>
+    <t>PJR20242484</t>
+  </si>
+  <si>
+    <t>SOWVF0202402</t>
+  </si>
+  <si>
+    <t>Dennis</t>
+  </si>
+  <si>
+    <t>9/26/2024</t>
+  </si>
+  <si>
+    <t>Cyber Security</t>
   </si>
 </sst>
 </file>
@@ -155,13 +140,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -443,10 +425,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O3"/>
+  <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -501,96 +483,48 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I2" t="b">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>2</v>
+      </c>
+      <c r="O2" t="s">
         <v>15</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="I2" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="J2" s="2">
-        <v>0</v>
-      </c>
-      <c r="K2" s="2">
-        <v>0</v>
-      </c>
-      <c r="L2" s="2">
-        <v>0</v>
-      </c>
-      <c r="M2" s="2">
-        <v>29</v>
-      </c>
-      <c r="N2" s="2">
-        <v>29</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="I3" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="J3" s="2">
-        <v>0</v>
-      </c>
-      <c r="K3" s="2">
-        <v>0</v>
-      </c>
-      <c r="L3" s="2">
-        <v>852147</v>
-      </c>
-      <c r="M3" s="2">
-        <v>67</v>
-      </c>
-      <c r="N3" s="2">
-        <v>67</v>
-      </c>
-      <c r="O3" s="2" t="s">
-        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>